<commit_message>
Update documentation with normalization options and clarify Experiment Setup CSV structure
</commit_message>
<xml_diff>
--- a/eln/development_roadmap.xlsx
+++ b/eln/development_roadmap.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.chitwood/code/sortscore/eln/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D495E28-5312-084F-A5A6-1D1C5B6B53FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30858CA-EE5B-2245-8230-861AF4DECF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{76BD3E29-AEC1-9147-B335-B8AB75B736A4}"/>
+    <workbookView minimized="1" xWindow="4080" yWindow="-360" windowWidth="30240" windowHeight="18880" xr2:uid="{76BD3E29-AEC1-9147-B335-B8AB75B736A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="OTX2_info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="139">
   <si>
     <t>Task</t>
   </si>
@@ -318,9 +318,6 @@
     <t>Development Stage 2: Normalization (across oligos, etc)</t>
   </si>
   <si>
-    <t>Development Stage 3: Document and Release</t>
-  </si>
-  <si>
     <t>Validate with existing GLI2 analysis</t>
   </si>
   <si>
@@ -445,6 +442,18 @@
   </si>
   <si>
     <t>before and after filtering</t>
+  </si>
+  <si>
+    <t>Development Stage 4: Test, Document and Release</t>
+  </si>
+  <si>
+    <t>Development Stage 3: Cleanup and Verify</t>
+  </si>
+  <si>
+    <t>Test on saturation mutagenesis dataset</t>
+  </si>
+  <si>
+    <t>Could I easily wrap my SLURM scripts to incorporate as an option?</t>
   </si>
 </sst>
 </file>
@@ -612,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -656,9 +665,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -669,9 +678,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,46 +812,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="7"/>
@@ -853,10 +846,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -893,6 +887,19 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="7"/>
@@ -924,6 +931,19 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="7"/>
@@ -953,6 +973,19 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -989,89 +1022,85 @@
 </FeaturePropertyBags>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2FFD0575-DC08-A24D-9C0F-3BDA617FCD56}" name="Table3" displayName="Table3" ref="A3:C19" totalsRowShown="0">
   <autoFilter ref="A3:C19" xr:uid="{2FFD0575-DC08-A24D-9C0F-3BDA617FCD56}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{100A207C-268C-2C4C-8C1D-81E5DC9AB42C}" name="Task" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{D453A652-1154-5844-8D72-7C31A9E34B10}" name="Status" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{BABB0024-F956-8B4B-86A3-233436F8DC71}" name="Notes" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{100A207C-268C-2C4C-8C1D-81E5DC9AB42C}" name="Task" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{D453A652-1154-5844-8D72-7C31A9E34B10}" name="Status" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{BABB0024-F956-8B4B-86A3-233436F8DC71}" name="Notes" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{798A5E2B-40D6-9D4C-84F5-A6511694C231}" name="Table2" displayName="Table2" ref="A59:C65" totalsRowShown="0" headerRowDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{798A5E2B-40D6-9D4C-84F5-A6511694C231}" name="Table2" displayName="Table2" ref="A59:C65" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A59:C65" xr:uid="{798A5E2B-40D6-9D4C-84F5-A6511694C231}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D5C9492D-F49F-4B49-A273-D526117E85C6}" name="Task" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{677AE15E-FF21-7849-918D-49558663DA01}" name="Status" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{961A6E6F-64C4-5B49-B9B4-B473C1CE3D3D}" name="Notes" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{D5C9492D-F49F-4B49-A273-D526117E85C6}" name="Task" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{677AE15E-FF21-7849-918D-49558663DA01}" name="Status" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{961A6E6F-64C4-5B49-B9B4-B473C1CE3D3D}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AE6226A0-FE58-534A-9CFF-FD2C4EE9660D}" name="Table4" displayName="Table4" ref="A22:C39" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AE6226A0-FE58-534A-9CFF-FD2C4EE9660D}" name="Table4" displayName="Table4" ref="A22:C39" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="A22:C39" xr:uid="{AE6226A0-FE58-534A-9CFF-FD2C4EE9660D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F14480B0-A263-BD4D-A97F-AC36A380228E}" name="Task" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{4D47C543-D845-B843-B093-B1DDFC283CF0}" name="Status" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{746AD611-AFFD-7645-A4CD-CF82C2A9BF93}" name="Notes" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{F14480B0-A263-BD4D-A97F-AC36A380228E}" name="Task" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{4D47C543-D845-B843-B093-B1DDFC283CF0}" name="Status" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{746AD611-AFFD-7645-A4CD-CF82C2A9BF93}" name="Notes" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9C3668F8-280D-CC47-A29A-642A1416A5DF}" name="Table26" displayName="Table26" ref="A94:C102" totalsRowShown="0" headerRowDxfId="28" tableBorderDxfId="27">
-  <autoFilter ref="A94:C102" xr:uid="{9C3668F8-280D-CC47-A29A-642A1416A5DF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9C3668F8-280D-CC47-A29A-642A1416A5DF}" name="Table26" displayName="Table26" ref="A101:C109" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
+  <autoFilter ref="A101:C109" xr:uid="{9C3668F8-280D-CC47-A29A-642A1416A5DF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{037554E1-3F64-F34E-8F31-D978A4EB2973}" name="Task" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{E0AB5D01-A5FC-8F49-A2A9-7227BEB9816B}" name="Status" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{3BBC3F43-C9D8-924B-970D-B511DEDB42D6}" name="Notes" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{037554E1-3F64-F34E-8F31-D978A4EB2973}" name="Task" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{E0AB5D01-A5FC-8F49-A2A9-7227BEB9816B}" name="Status" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{3BBC3F43-C9D8-924B-970D-B511DEDB42D6}" name="Notes" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{451C9632-D621-594C-A465-A459EAAA8C64}" name="Table262" displayName="Table262" ref="A81:C91" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="A81:C91" xr:uid="{451C9632-D621-594C-A465-A459EAAA8C64}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{451C9632-D621-594C-A465-A459EAAA8C64}" name="Table262" displayName="Table262" ref="A88:C98" totalsRowShown="0" headerRowDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="A88:C98" xr:uid="{451C9632-D621-594C-A465-A459EAAA8C64}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{367A0B47-309E-3142-8989-FEA007CE7904}" name="Task" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{B8F1DF19-5512-0642-8A3B-985309489837}" name="Status" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{C17E4518-574D-B24D-9143-A4D578986D22}" name="Notes" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{367A0B47-309E-3142-8989-FEA007CE7904}" name="Task" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{B8F1DF19-5512-0642-8A3B-985309489837}" name="Status" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{C17E4518-574D-B24D-9143-A4D578986D22}" name="Notes" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1A214C12-09B8-F641-81FD-70CAF57E1615}" name="Table28" displayName="Table28" ref="A68:C78" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A68:C78" xr:uid="{1A214C12-09B8-F641-81FD-70CAF57E1615}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1A214C12-09B8-F641-81FD-70CAF57E1615}" name="Table28" displayName="Table28" ref="A75:C85" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A75:C85" xr:uid="{1A214C12-09B8-F641-81FD-70CAF57E1615}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F30F0003-37BA-EB4F-863B-2D053DA73144}" name="Task" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{9E038F0E-80BE-D447-9433-0BA72A8EC717}" name="Status" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{14A9CA77-D3D9-E14C-AA3C-08AEFD8DB224}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{F30F0003-37BA-EB4F-863B-2D053DA73144}" name="Task" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{9E038F0E-80BE-D447-9433-0BA72A8EC717}" name="Status" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{14A9CA77-D3D9-E14C-AA3C-08AEFD8DB224}" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FCD382CC-8BAB-E446-8E04-8555DB2C9612}" name="Table49" displayName="Table49" ref="A42:C56" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FCD382CC-8BAB-E446-8E04-8555DB2C9612}" name="Table49" displayName="Table49" ref="A42:C56" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A42:C56" xr:uid="{FCD382CC-8BAB-E446-8E04-8555DB2C9612}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E3B17CB0-1847-E14D-8BA9-67A3028DB203}" name="Task" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{053609AD-9098-6249-9D66-B8703F6109FD}" name="Status" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{5745B50A-E022-7645-8565-B5881B59EEBA}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E3B17CB0-1847-E14D-8BA9-67A3028DB203}" name="Task" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{053609AD-9098-6249-9D66-B8703F6109FD}" name="Status" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{5745B50A-E022-7645-8565-B5881B59EEBA}" name="Notes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1394,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABBC9CA-9B77-AB4C-9BA6-BBA8D09EAD80}">
-  <dimension ref="A1:M102"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,7 +1453,7 @@
     </row>
     <row r="2" spans="1:3" ht="22" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1510,7 +1539,7 @@
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="1" t="b">
         <v>1</v>
@@ -1518,7 +1547,7 @@
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1" t="b">
         <v>1</v>
@@ -1532,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1548,7 +1577,7 @@
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="1" t="b">
         <v>1</v>
@@ -1556,7 +1585,7 @@
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="1" t="b">
         <v>1</v>
@@ -1564,18 +1593,18 @@
     </row>
     <row r="18" spans="1:3" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="1" t="b">
         <v>1</v>
@@ -1586,7 +1615,7 @@
     </row>
     <row r="21" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1695,7 +1724,7 @@
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" s="1" t="b">
         <v>0</v>
@@ -1710,8 +1739,8 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
-        <v>103</v>
+      <c r="A34" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="B34" s="1" t="b">
         <v>0</v>
@@ -1742,7 +1771,7 @@
     </row>
     <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B37" s="1" t="b">
         <v>0</v>
@@ -1751,7 +1780,7 @@
     </row>
     <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B38" s="1" t="b">
         <v>0</v>
@@ -1768,7 +1797,7 @@
     </row>
     <row r="41" spans="1:13" ht="24" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1790,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1801,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1812,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1854,7 +1883,7 @@
     </row>
     <row r="50" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B50" s="2" t="b">
         <v>0</v>
@@ -1874,7 +1903,7 @@
     </row>
     <row r="52" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B52" s="1" t="b">
         <v>0</v>
@@ -1882,7 +1911,7 @@
     </row>
     <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B53" s="1" t="b">
         <v>0</v>
@@ -1890,19 +1919,19 @@
     </row>
     <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="B54" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="M54" s="5"/>
     </row>
     <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B55" s="1" t="b">
         <v>0</v>
@@ -1911,7 +1940,7 @@
     </row>
     <row r="56" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B56" s="1" t="b">
         <v>0</v>
@@ -1953,13 +1982,13 @@
     </row>
     <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="B62" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1980,7 +2009,7 @@
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65" s="1" t="b">
         <v>0</v>
@@ -1988,7 +2017,7 @@
     </row>
     <row r="67" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2003,272 +2032,318 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B69" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B70" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B71" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B72" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B73" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B74" s="1" t="b">
-        <v>0</v>
+      <c r="A69" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C69" s="22"/>
+    </row>
+    <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C70" s="22"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="23"/>
+      <c r="B71" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C71" s="25"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="20"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="22"/>
+    </row>
+    <row r="74" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A74" s="13" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B75" s="1" t="b">
-        <v>0</v>
+      <c r="A75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B76" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="B77" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="B78" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="25" x14ac:dyDescent="0.3">
-      <c r="A80" s="9" t="s">
-        <v>77</v>
+    <row r="79" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A79" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B80" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>2</v>
+      <c r="A81" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="B82" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="B83" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B84" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C84" s="19"/>
-    </row>
-    <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
-        <v>81</v>
-      </c>
+      <c r="A84" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B86" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B87" s="1" t="b">
-        <v>0</v>
+    <row r="87" spans="1:3" ht="25" x14ac:dyDescent="0.3">
+      <c r="A87" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B88" s="1" t="b">
-        <v>0</v>
+      <c r="A88" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B89" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="B90" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="25" x14ac:dyDescent="0.3">
-      <c r="A93" s="9" t="s">
-        <v>68</v>
+      <c r="A91" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B91" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C91" s="19"/>
+    </row>
+    <row r="92" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="18" t="s">
-        <v>2</v>
+      <c r="A94" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B94" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B95" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C95" s="19"/>
+      <c r="A95" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B95" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B96" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B97" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="25" x14ac:dyDescent="0.3">
+      <c r="A100" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C102" s="19"/>
+    </row>
+    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A105" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A106" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B98" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A99" s="8" t="s">
+      <c r="B106" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B99" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C99" s="8" t="s">
+    </row>
+    <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B107" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B108" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="8" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A100" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B100" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B101" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B102" s="1" t="b">
+      <c r="B109" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>